<commit_message>
unit conversion for RC Sections
</commit_message>
<xml_diff>
--- a/m100_Tools_And_Helpers/DataFiles/RC Section Definitions.xlsx
+++ b/m100_Tools_And_Helpers/DataFiles/RC Section Definitions.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\repos\LusasNoteBooks\m100_Tools_And_Helpers\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E04BA99-CB91-4CF4-B992-B10EA08D655C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A591ACA-80F4-405A-BF61-5A2AFD0AA38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7DE9D511-3767-4F7D-816D-88B9A9290805}"/>
+    <workbookView xWindow="28680" yWindow="1620" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{7DE9D511-3767-4F7D-816D-88B9A9290805}"/>
   </bookViews>
   <sheets>
     <sheet name="Rectangular" sheetId="1" r:id="rId1"/>
     <sheet name="Tee" sheetId="2" r:id="rId2"/>
+    <sheet name="Circular" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -45,9 +46,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>SI</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -109,6 +107,21 @@
   </si>
   <si>
     <t>3x25|3x20</t>
+  </si>
+  <si>
+    <t>Column 400dia</t>
+  </si>
+  <si>
+    <t>10x25</t>
+  </si>
+  <si>
+    <t>15x25|10x20</t>
+  </si>
+  <si>
+    <t>N,mm,t,s,C</t>
+  </si>
+  <si>
+    <t>Column 500dia, 2layers</t>
   </si>
 </sst>
 </file>
@@ -500,13 +513,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F08E83C-9C4E-4F8F-8B22-77E004008076}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -517,33 +531,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2">
         <v>400</v>
@@ -555,23 +569,25 @@
         <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C3" s="2">
         <v>300</v>
       </c>
@@ -582,11 +598,11 @@
         <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -597,15 +613,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0B5071-37E8-4339-9FD5-4CB7091DBCBC}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -617,53 +634,55 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C2" s="2">
         <v>1000</v>
       </c>
@@ -683,16 +702,90 @@
         <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108B640C-5711-4769-9E84-6450DFA13967}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2">
+        <v>400</v>
+      </c>
+      <c r="D2" s="2">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2">
+        <v>500</v>
+      </c>
+      <c r="D3" s="2">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>